<commit_message>
made edits to planning files. exported planning data files to PDFs and PNGs.
</commit_message>
<xml_diff>
--- a/planning/record_shop_activity_gantt.xlsx
+++ b/planning/record_shop_activity_gantt.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="11560" yWindow="0" windowWidth="14200" windowHeight="17140" tabRatio="500"/>
   </bookViews>
@@ -115,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +137,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -505,7 +511,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -685,7 +691,12 @@
       <c r="H21" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="9" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>